<commit_message>
Fix issue with SS on score and Internal server error on other profiles
</commit_message>
<xml_diff>
--- a/trail.xlsx
+++ b/trail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Negative tweets:</t>
   </si>
@@ -32,25 +32,13 @@
   </si>
   <si>
     <t>tweet</t>
-  </si>
-  <si>
-    <t>Jul 07 2017</t>
-  </si>
-  <si>
-    <t>negative</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/885161449018073088</t>
-  </si>
-  <si>
-    <t>RT @jasonmashak: Yes, it's obvious, unfortunate &amp;amp; unfair. We in the security industry have great respect for @e_kaspersky's contributions t…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,14 +50,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,10 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,27 +400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>-0.04999999999999999</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>